<commit_message>
Atualização do dicionário de dados
</commit_message>
<xml_diff>
--- a/documentacao/Dicionario.xlsx
+++ b/documentacao/Dicionario.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizh.FEITOZA\Desktop\Luiz\Tecnico\Modulo 3\PRW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\VertrigoServ\www\ChatSchool\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E811ADDC-58D3-400D-B21F-5473491B8FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6870" yWindow="1500" windowWidth="14265" windowHeight="13530" xr2:uid="{769BFCCA-C7B9-4DC1-AD01-A20E028599FC}"/>
+    <workbookView xWindow="-6870" yWindow="1500" windowWidth="14265" windowHeight="13530"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="62">
   <si>
     <t>Nome</t>
   </si>
@@ -123,9 +122,6 @@
     <t>data_post</t>
   </si>
   <si>
-    <t>hora_post</t>
-  </si>
-  <si>
     <t>cod_like</t>
   </si>
   <si>
@@ -168,9 +164,6 @@
     <t>modulo_ano</t>
   </si>
   <si>
-    <t>COMUNICADO</t>
-  </si>
-  <si>
     <t>cod_comunicado</t>
   </si>
   <si>
@@ -211,12 +204,18 @@
   </si>
   <si>
     <t>destinatario</t>
+  </si>
+  <si>
+    <t>COMUNICADOS</t>
+  </si>
+  <si>
+    <t>data_comunicado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -386,11 +385,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,20 +410,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,99 +724,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF998D28-0229-4351-8F36-F753D088D655}">
-  <dimension ref="B4:BS42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:BM42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.85546875" customWidth="1"/>
-    <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.85546875" customWidth="1"/>
-    <col min="40" max="40" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="10.85546875" customWidth="1"/>
-    <col min="47" max="47" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.85546875" customWidth="1"/>
-    <col min="54" max="54" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.85546875" customWidth="1"/>
-    <col min="61" max="61" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" customWidth="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.85546875" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.85546875" customWidth="1"/>
+    <col min="48" max="48" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.85546875" customWidth="1"/>
+    <col min="55" max="55" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:60" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:54" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="H4" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-      <c r="N4" s="21" t="s">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="H4" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="23"/>
-      <c r="T4" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Z4" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA4" s="19"/>
-      <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AF4" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG4" s="19"/>
-      <c r="AH4" s="19"/>
-      <c r="AI4" s="19"/>
-      <c r="AJ4" s="19"/>
-    </row>
-    <row r="5" spans="2:60" x14ac:dyDescent="0.25">
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="28"/>
+      <c r="N4" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="T4" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Z4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+    </row>
+    <row r="5" spans="2:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
@@ -896,23 +881,8 @@
       <c r="AD5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AF5" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ5" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:60" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:54" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
@@ -928,7 +898,7 @@
       </c>
       <c r="G6"/>
       <c r="H6" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>11</v>
@@ -941,12 +911,12 @@
         <v>12</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="7"/>
+      <c r="P6" s="6"/>
       <c r="Q6" s="7" t="s">
         <v>6</v>
       </c>
@@ -954,20 +924,21 @@
         <v>12</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="U6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="V6" s="6"/>
+      <c r="V6" s="7"/>
       <c r="W6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="Y6" s="10"/>
       <c r="Z6" s="6" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="AA6" s="6" t="s">
         <v>11</v>
@@ -976,29 +947,15 @@
       <c r="AC6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AD6" s="7" t="s">
+      <c r="AD6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS6" s="10"/>
-      <c r="AZ6" s="10"/>
-      <c r="BG6" s="10"/>
-      <c r="BH6" s="5"/>
-    </row>
-    <row r="7" spans="2:60" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AM6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="5"/>
+    </row>
+    <row r="7" spans="2:54" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
@@ -1023,55 +980,44 @@
       </c>
       <c r="L7" s="6"/>
       <c r="N7" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7" t="s">
-        <v>10</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="P7" s="7">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="T7" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="U7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="11"/>
+      <c r="Z7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="V7" s="7">
-        <v>35</v>
-      </c>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Z7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="AB7" s="7">
+        <v>1000</v>
+      </c>
+      <c r="AC7" s="7"/>
       <c r="AD7" s="6"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH7" s="7">
-        <v>1000</v>
-      </c>
-      <c r="AI7" s="7"/>
-      <c r="AJ7" s="6"/>
-      <c r="AS7" s="11"/>
-      <c r="AZ7" s="11"/>
-      <c r="BG7" s="11"/>
-    </row>
-    <row r="8" spans="2:60" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AM7" s="11"/>
+      <c r="AT7" s="11"/>
+      <c r="BA7" s="11"/>
+    </row>
+    <row r="8" spans="2:54" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1084,56 +1030,45 @@
       <c r="E8" s="7"/>
       <c r="F8" s="6"/>
       <c r="G8"/>
-      <c r="H8" s="16" t="s">
-        <v>24</v>
+      <c r="H8" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="8"/>
-      <c r="N8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="7">
+      <c r="J8" s="7">
         <v>70</v>
       </c>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="T8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="V8" s="7">
+        <v>350</v>
+      </c>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="11"/>
       <c r="Z8" s="6" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="AA8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB8" s="7">
-        <v>350</v>
-      </c>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH8" s="7"/>
-      <c r="AI8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ8" s="6"/>
-      <c r="AS8" s="11"/>
-      <c r="AZ8" s="11"/>
-      <c r="BG8" s="11"/>
-    </row>
-    <row r="9" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD8" s="6"/>
+      <c r="AM8" s="11"/>
+      <c r="AT8" s="11"/>
+      <c r="BA8" s="11"/>
+    </row>
+    <row r="9" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
@@ -1146,27 +1081,36 @@
       <c r="E9" s="7"/>
       <c r="F9" s="6"/>
       <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9" s="12"/>
-      <c r="N9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="6"/>
-      <c r="T9" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="6"/>
+      <c r="N9" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="T9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="13"/>
       <c r="Z9" s="6" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="AA9" s="6" t="s">
         <v>11</v>
@@ -1176,23 +1120,11 @@
         <v>10</v>
       </c>
       <c r="AD9" s="6"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH9" s="7"/>
-      <c r="AI9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ9" s="6"/>
-      <c r="AS9" s="12"/>
-      <c r="AZ9" s="12"/>
-      <c r="BG9" s="12"/>
-    </row>
-    <row r="10" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM9" s="12"/>
+      <c r="AT9" s="12"/>
+      <c r="BA9" s="12"/>
+    </row>
+    <row r="10" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
@@ -1207,57 +1139,50 @@
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
-      <c r="J10" s="12"/>
-      <c r="N10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="6"/>
-      <c r="T10" s="8" t="s">
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="N10" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="U10" s="8" t="s">
+      <c r="O10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="V10" s="8" t="s">
+      <c r="P10" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="W10" s="8" t="s">
+      <c r="Q10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="X10" s="8" t="s">
+      <c r="R10" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="T10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="13"/>
       <c r="Z10" s="6" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="AA10" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AB10" s="7"/>
-      <c r="AC10" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="AC10" s="7"/>
       <c r="AD10" s="6"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH10" s="7"/>
-      <c r="AI10" s="7"/>
-      <c r="AJ10" s="6"/>
-      <c r="AS10" s="13"/>
-      <c r="AZ10" s="13"/>
-      <c r="BG10" s="13"/>
-    </row>
-    <row r="11" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="BA10" s="13"/>
+    </row>
+    <row r="11" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1268,51 +1193,51 @@
       <c r="E11" s="7"/>
       <c r="F11" s="6"/>
       <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-      <c r="R11"/>
+      <c r="H11" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="N11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="T11" s="6" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="U11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="V11" s="6"/>
+      <c r="V11" s="7"/>
       <c r="W11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X11" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="X11" s="6"/>
       <c r="Z11" s="6" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="AA11" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AB11" s="7"/>
-      <c r="AC11" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="AC11" s="7"/>
       <c r="AD11" s="6"/>
-      <c r="AF11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="7"/>
-      <c r="AJ11" s="6"/>
-      <c r="AS11" s="13"/>
-      <c r="AZ11" s="13"/>
-      <c r="BG11" s="13"/>
-    </row>
-    <row r="12" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AM11" s="13"/>
+      <c r="AT11" s="13"/>
+      <c r="BA11" s="13"/>
+    </row>
+    <row r="12" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
@@ -1325,37 +1250,47 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="N12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="T12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="U12" s="6" t="s">
+      <c r="H12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="7">
+      <c r="P12" s="7">
         <v>50</v>
       </c>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AR12" s="13"/>
-      <c r="AS12" s="13"/>
-      <c r="AZ12" s="13"/>
-      <c r="BG12" s="13"/>
-    </row>
-    <row r="13" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="T12" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="U12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="AL12" s="13"/>
+      <c r="AM12" s="13"/>
+      <c r="AT12" s="13"/>
+      <c r="BA12" s="13"/>
+    </row>
+    <row r="13" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
@@ -1368,34 +1303,25 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
       <c r="G13"/>
-      <c r="N13" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="O13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="R13" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z13" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
-      <c r="AC13" s="19"/>
-      <c r="AD13" s="19"/>
-      <c r="AR13" s="13"/>
-      <c r="AS13" s="13"/>
-      <c r="AZ13" s="13"/>
-      <c r="BG13" s="13"/>
-    </row>
-    <row r="14" spans="2:60" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL13" s="13"/>
+      <c r="AM13" s="13"/>
+      <c r="AT13" s="13"/>
+      <c r="BA13" s="13"/>
+    </row>
+    <row r="14" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>21</v>
       </c>
@@ -1408,47 +1334,37 @@
       <c r="E14" s="7"/>
       <c r="F14" s="6"/>
       <c r="G14"/>
-      <c r="N14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="T14" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="U14" s="22"/>
-      <c r="V14" s="22"/>
-      <c r="W14" s="22"/>
-      <c r="X14" s="23"/>
-      <c r="Z14" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB14" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC14" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD14" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="AR14" s="13"/>
-      <c r="AS14" s="13"/>
-      <c r="AZ14" s="13"/>
-      <c r="BG14" s="13"/>
-    </row>
-    <row r="15" spans="2:60" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="H14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="N14" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
+      <c r="Q14" s="27"/>
+      <c r="R14" s="28"/>
+      <c r="T14" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="AL14" s="13"/>
+      <c r="AM14" s="13"/>
+      <c r="AT14" s="13"/>
+      <c r="BA14" s="13"/>
+    </row>
+    <row r="15" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
@@ -1458,17 +1374,32 @@
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
       <c r="F15" s="6"/>
-      <c r="N15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="R15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="N15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="T15" s="8" t="s">
         <v>0</v>
       </c>
@@ -1484,37 +1415,31 @@
       <c r="X15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Z15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL15" s="13"/>
-      <c r="AZ15" s="13"/>
-      <c r="BG15" s="13"/>
-    </row>
-    <row r="16" spans="2:60" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="AF15" s="13"/>
+      <c r="AT15" s="13"/>
+      <c r="BA15" s="13"/>
+    </row>
+    <row r="16" spans="2:54" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
       <c r="N16" s="6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="O16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="P16" s="7"/>
       <c r="Q16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="R16" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="T16" s="6" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="U16" s="6" t="s">
         <v>11</v>
@@ -1526,266 +1451,307 @@
       <c r="X16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Z16" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA16" s="25" t="s">
+      <c r="AF16" s="13"/>
+    </row>
+    <row r="17" spans="2:65" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="H17" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="N17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" s="7">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="T17" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="U17" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AB16" s="26"/>
-      <c r="AC16" s="26"/>
-      <c r="AD16" s="25"/>
-      <c r="AL16" s="13"/>
-    </row>
-    <row r="17" spans="2:71" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="N17"/>
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
-      <c r="R17"/>
-      <c r="T17" s="6" t="s">
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="21"/>
+      <c r="BL17" s="14"/>
+      <c r="BM17" s="14"/>
+    </row>
+    <row r="18" spans="2:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R18" s="6"/>
+      <c r="T18" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="V18" s="7">
+        <v>50</v>
+      </c>
+      <c r="W18" s="7"/>
+      <c r="X18" s="6"/>
+      <c r="BL18" s="15"/>
+      <c r="BM18" s="15"/>
+    </row>
+    <row r="19" spans="2:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="U17" s="6" t="s">
+      <c r="O19" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="V17" s="7">
-        <v>3</v>
-      </c>
-      <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Z17" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA17" s="6" t="s">
+      <c r="P19" s="7">
         <v>5</v>
       </c>
-      <c r="AB17" s="7">
-        <v>50</v>
-      </c>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="6"/>
-      <c r="BR17" s="14"/>
-      <c r="BS17" s="14"/>
-    </row>
-    <row r="18" spans="2:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N18" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
-      <c r="T18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="X18" s="6"/>
-      <c r="Z18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA18" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB18" s="27"/>
-      <c r="AC18" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD18" s="17"/>
-      <c r="BR18" s="15"/>
-      <c r="BS18" s="15"/>
-    </row>
-    <row r="19" spans="2:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N19" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="O19" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="P19" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q19" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="R19" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="T19" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="U19" s="24" t="s">
+      <c r="Q19" s="7"/>
+      <c r="R19" s="17"/>
+      <c r="BL19" s="15"/>
+      <c r="BM19" s="15"/>
+    </row>
+    <row r="20" spans="2:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="V19" s="7">
-        <v>5</v>
-      </c>
-      <c r="W19" s="7"/>
-      <c r="X19" s="17"/>
-      <c r="BR19" s="15"/>
-      <c r="BS19" s="15"/>
-    </row>
-    <row r="20" spans="2:71" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="N20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O20" s="6" t="s">
+      <c r="J20" s="7">
+        <v>280</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="6"/>
+      <c r="N20" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="O20" s="20" t="s">
         <v>11</v>
       </c>
       <c r="P20" s="7"/>
       <c r="Q20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="R20" s="17"/>
+      <c r="T20" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="25"/>
+      <c r="X20" s="25"/>
+      <c r="BL20" s="15"/>
+      <c r="BM20" s="15"/>
+    </row>
+    <row r="21" spans="2:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="H21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="6"/>
+      <c r="N21" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="T21" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="V21" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="W21" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="X21" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL21" s="15"/>
+      <c r="BM21" s="15"/>
+    </row>
+    <row r="22" spans="2:65" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="6"/>
+      <c r="T22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="T20" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="U20" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="X20" s="17"/>
-      <c r="Z20" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA20" s="19"/>
-      <c r="AB20" s="19"/>
-      <c r="AC20" s="19"/>
-      <c r="AD20" s="19"/>
-      <c r="BR20" s="15"/>
-      <c r="BS20" s="15"/>
-    </row>
-    <row r="21" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="N21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="P21" s="7">
-        <v>280</v>
-      </c>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="6"/>
-      <c r="T21" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="U21" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="V21" s="17"/>
-      <c r="W21" s="17"/>
-      <c r="X21" s="17"/>
-      <c r="Z21" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="AC21" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD21" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="BR21" s="15"/>
-      <c r="BS21" s="15"/>
-    </row>
-    <row r="22" spans="2:71" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="N22" s="6" t="s">
+      <c r="X22" s="18"/>
+      <c r="BL22" s="15"/>
+      <c r="BM22" s="15"/>
+    </row>
+    <row r="23" spans="2:65" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="U23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V23" s="24"/>
+      <c r="W23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X23" s="8"/>
+      <c r="BL23" s="15"/>
+      <c r="BM23" s="15"/>
+    </row>
+    <row r="24" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="T24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="O22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="R22" s="6"/>
-      <c r="Z22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB22" s="7"/>
-      <c r="AC22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD22" s="18"/>
-      <c r="BR22" s="15"/>
-      <c r="BS22" s="15"/>
-    </row>
-    <row r="23" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="N23" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="R23" s="6"/>
-      <c r="Z23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB23" s="29"/>
-      <c r="AC23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD23" s="8"/>
-      <c r="BR23" s="15"/>
-      <c r="BS23" s="15"/>
-    </row>
-    <row r="24" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="Z24" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD24" s="6"/>
-      <c r="BR24" s="15"/>
-      <c r="BS24" s="15"/>
-    </row>
-    <row r="25" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="BR25" s="15"/>
-      <c r="BS25" s="15"/>
-    </row>
-    <row r="26" spans="2:71" x14ac:dyDescent="0.25">
-      <c r="BR26" s="15"/>
-      <c r="BS26" s="15"/>
-    </row>
-    <row r="27" spans="2:71" x14ac:dyDescent="0.25">
+      <c r="U24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="V24" s="6"/>
+      <c r="W24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="X24" s="6"/>
+      <c r="BL24" s="15"/>
+      <c r="BM24" s="15"/>
+    </row>
+    <row r="25" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BL25" s="15"/>
+      <c r="BM25" s="15"/>
+    </row>
+    <row r="26" spans="2:65" x14ac:dyDescent="0.25">
+      <c r="BL26" s="15"/>
+      <c r="BM26" s="15"/>
+    </row>
+    <row r="27" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
-      <c r="BR27" s="15"/>
-      <c r="BS27" s="15"/>
-    </row>
-    <row r="30" spans="2:71" x14ac:dyDescent="0.25">
+      <c r="BL27" s="15"/>
+      <c r="BM27" s="15"/>
+    </row>
+    <row r="30" spans="2:65" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -1805,18 +1771,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="AF4:AJ4"/>
     <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="Z13:AD13"/>
-    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="T4:X4"/>
     <mergeCell ref="T14:X14"/>
-    <mergeCell ref="T9:X9"/>
-    <mergeCell ref="Z20:AD20"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="T20:X20"/>
     <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B17:F17"/>
     <mergeCell ref="H4:L4"/>
+    <mergeCell ref="H11:L11"/>
     <mergeCell ref="N4:R4"/>
-    <mergeCell ref="N12:R12"/>
-    <mergeCell ref="T4:X4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>